<commit_message>
now the one before the last
</commit_message>
<xml_diff>
--- a/summary/readme.xlsx
+++ b/summary/readme.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-4332" yWindow="9648" windowWidth="28800" windowHeight="13572"/>
+    <workbookView xWindow="1480" yWindow="0" windowWidth="25600" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>class 1</t>
   </si>
@@ -245,17 +245,33 @@
   </si>
   <si>
     <t>graph 11</t>
+  </si>
+  <si>
+    <t>797 left undone</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>140 pure backtracking with memoization passed, but lack a dp solution</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>752 left undone</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hw: 269</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -263,7 +279,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -271,21 +287,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -293,7 +309,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -302,7 +318,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -310,7 +326,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -387,27 +403,27 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="21">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Good" xfId="3" builtinId="26"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="3" builtinId="26"/>
+    <cellStyle name="差" xfId="2" builtinId="27"/>
+    <cellStyle name="无色" xfId="4" builtinId="28"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="标题 1" xfId="1" builtinId="16"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -465,7 +481,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,7 +516,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -711,13 +727,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="40.109375" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" customWidth="1"/>
     <col min="9" max="9" width="25.33203125" customWidth="1"/>
     <col min="12" max="12" width="23.33203125" customWidth="1"/>
@@ -842,7 +858,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="15.6">
+    <row r="2" spans="1:39" ht="15">
       <c r="A2">
         <v>27</v>
       </c>
@@ -961,7 +977,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="15.6">
+    <row r="3" spans="1:39" ht="15">
       <c r="A3">
         <v>26</v>
       </c>
@@ -1080,7 +1096,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="15.6">
+    <row r="4" spans="1:39" ht="15">
       <c r="A4">
         <v>80</v>
       </c>
@@ -1293,14 +1309,17 @@
       <c r="AH5">
         <v>23</v>
       </c>
-      <c r="AI5">
+      <c r="AI5" s="4">
         <v>797</v>
       </c>
       <c r="AJ5">
         <v>46</v>
       </c>
-      <c r="AK5">
+      <c r="AK5" s="4">
         <v>752</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:39">
@@ -1615,6 +1634,9 @@
       <c r="Z10">
         <v>439</v>
       </c>
+      <c r="AI10" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" spans="1:39">
       <c r="C11">
@@ -1638,6 +1660,9 @@
       <c r="V11">
         <v>590</v>
       </c>
+      <c r="AI11" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="12" spans="1:39">
       <c r="C12">
@@ -1649,6 +1674,9 @@
       <c r="I12">
         <v>227</v>
       </c>
+      <c r="AI12" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="13" spans="1:39">
       <c r="C13">
@@ -1679,7 +1707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="20.399999999999999" thickBot="1">
+    <row r="21" spans="1:7" ht="19" thickBot="1">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>

</xml_diff>